<commit_message>
Comparing PCA methods and using biomaRt and clusterProfiler need to be done
</commit_message>
<xml_diff>
--- a/BulkRNA-seq/Project_CL-Treatment/Resources/RData/sig_lfc_res_FC15.xlsx
+++ b/BulkRNA-seq/Project_CL-Treatment/Resources/RData/sig_lfc_res_FC15.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jigsaw-0/Workspace/SNU-BIOINFO/Dojo/BI-dojo/BulkRNA-seq/Project_CL-Treatment/Resources/RData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C236B8E0-1AC5-904D-A16A-2A8D67C56FF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81225038-CC30-7744-AAE5-277B4DDE0D6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="760" windowWidth="26700" windowHeight="16500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7583,8 +7583,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F2381"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1446" workbookViewId="0">
-      <selection activeCell="K1472" sqref="K1472"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -55216,5 +55216,6 @@
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>